<commit_message>
Function for generating X data
</commit_message>
<xml_diff>
--- a/dataforfinalproject/RawDataFiles/Codebooks/Codebook_allyears.xlsx
+++ b/dataforfinalproject/RawDataFiles/Codebooks/Codebook_allyears.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SMU DS Bootcamp\Projects\Project3-ML_ResPoweConsumption\Project3final\dataforfinalproject\RawDataFiles\Codebooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2F5220B-03A2-450D-A320-43CF8A528D26}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48DB71A6-574F-4CE9-9D93-46CA070BA9F0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930" activeTab="4" xr2:uid="{D5B27A2C-9AC0-4372-9500-4C3681F36C9F}"/>
   </bookViews>
@@ -20228,7 +20228,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="23" x14ac:knownFonts="1">
+  <fonts count="25" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -20394,6 +20394,20 @@
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="35">
@@ -20766,7 +20780,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -20809,6 +20823,14 @@
     <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -21031,7 +21053,7 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="50">
     <cellStyle name="20% - Accent1" xfId="17" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="20" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="23" builtinId="38" customBuiltin="1"/>
@@ -21044,11 +21066,17 @@
     <cellStyle name="40% - Accent4" xfId="27" builtinId="43" customBuiltin="1"/>
     <cellStyle name="40% - Accent5" xfId="30" builtinId="47" customBuiltin="1"/>
     <cellStyle name="40% - Accent6" xfId="33" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="44" builtinId="32" customBuiltin="1"/>
     <cellStyle name="60% - Accent1 2" xfId="36" xr:uid="{00000000-0005-0000-0000-00002F000000}"/>
+    <cellStyle name="60% - Accent2" xfId="45" builtinId="36" customBuiltin="1"/>
     <cellStyle name="60% - Accent2 2" xfId="37" xr:uid="{00000000-0005-0000-0000-000030000000}"/>
+    <cellStyle name="60% - Accent3" xfId="46" builtinId="40" customBuiltin="1"/>
     <cellStyle name="60% - Accent3 2" xfId="38" xr:uid="{00000000-0005-0000-0000-000031000000}"/>
+    <cellStyle name="60% - Accent4" xfId="47" builtinId="44" customBuiltin="1"/>
     <cellStyle name="60% - Accent4 2" xfId="39" xr:uid="{00000000-0005-0000-0000-000032000000}"/>
+    <cellStyle name="60% - Accent5" xfId="48" builtinId="48" customBuiltin="1"/>
     <cellStyle name="60% - Accent5 2" xfId="40" xr:uid="{00000000-0005-0000-0000-000033000000}"/>
+    <cellStyle name="60% - Accent6" xfId="49" builtinId="52" customBuiltin="1"/>
     <cellStyle name="60% - Accent6 2" xfId="41" xr:uid="{00000000-0005-0000-0000-000034000000}"/>
     <cellStyle name="Accent1" xfId="16" builtinId="29" customBuiltin="1"/>
     <cellStyle name="Accent2" xfId="19" builtinId="33" customBuiltin="1"/>
@@ -21067,10 +21095,12 @@
     <cellStyle name="Heading 4" xfId="4" builtinId="19" customBuiltin="1"/>
     <cellStyle name="Input" xfId="7" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="10" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="43" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Neutral 2" xfId="35" xr:uid="{00000000-0005-0000-0000-000035000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="13" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Output" xfId="8" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="42" builtinId="15" customBuiltin="1"/>
     <cellStyle name="Title 2" xfId="34" xr:uid="{00000000-0005-0000-0000-000036000000}"/>
     <cellStyle name="Total" xfId="15" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="12" builtinId="11" customBuiltin="1"/>
@@ -53230,8 +53260,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8288F514-4EDA-43BF-B0BC-9F0DDD252265}">
   <dimension ref="A1:F942"/>
   <sheetViews>
-    <sheetView topLeftCell="A603" workbookViewId="0">
-      <selection activeCell="F604" sqref="F604"/>
+    <sheetView topLeftCell="A660" workbookViewId="0">
+      <selection activeCell="A665" sqref="A665"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -64396,7 +64426,7 @@
         <v>3852</v>
       </c>
     </row>
-    <row r="799" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="799" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A799" s="31" t="s">
         <v>4960</v>
       </c>
@@ -64438,7 +64468,7 @@
         <v>3852</v>
       </c>
     </row>
-    <row r="802" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="802" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A802" s="31" t="s">
         <v>4965</v>
       </c>
@@ -64452,7 +64482,7 @@
         <v>3852</v>
       </c>
     </row>
-    <row r="803" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="803" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A803" s="31" t="s">
         <v>4967</v>
       </c>
@@ -64466,7 +64496,7 @@
         <v>3852</v>
       </c>
     </row>
-    <row r="804" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="804" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A804" s="31" t="s">
         <v>4969</v>
       </c>
@@ -64480,7 +64510,7 @@
         <v>3852</v>
       </c>
     </row>
-    <row r="805" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="805" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A805" s="31" t="s">
         <v>4971</v>
       </c>
@@ -64494,7 +64524,7 @@
         <v>3852</v>
       </c>
     </row>
-    <row r="806" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="806" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A806" s="31" t="s">
         <v>4973</v>
       </c>
@@ -64508,7 +64538,7 @@
         <v>3852</v>
       </c>
     </row>
-    <row r="807" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="807" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A807" s="31" t="s">
         <v>4975</v>
       </c>
@@ -64522,7 +64552,7 @@
         <v>3852</v>
       </c>
     </row>
-    <row r="808" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="808" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A808" s="31" t="s">
         <v>4977</v>
       </c>
@@ -64536,7 +64566,7 @@
         <v>3852</v>
       </c>
     </row>
-    <row r="809" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="809" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A809" s="31" t="s">
         <v>4979</v>
       </c>
@@ -64550,7 +64580,7 @@
         <v>3852</v>
       </c>
     </row>
-    <row r="810" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="810" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A810" s="31" t="s">
         <v>4981</v>
       </c>
@@ -64564,7 +64594,7 @@
         <v>3852</v>
       </c>
     </row>
-    <row r="811" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="811" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A811" s="31" t="s">
         <v>4983</v>
       </c>
@@ -64578,7 +64608,7 @@
         <v>3852</v>
       </c>
     </row>
-    <row r="812" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="812" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A812" s="31" t="s">
         <v>4985</v>
       </c>
@@ -64592,7 +64622,7 @@
         <v>3852</v>
       </c>
     </row>
-    <row r="813" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="813" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A813" s="31" t="s">
         <v>4987</v>
       </c>
@@ -64606,7 +64636,7 @@
         <v>3852</v>
       </c>
     </row>
-    <row r="814" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="814" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A814" s="31" t="s">
         <v>4989</v>
       </c>
@@ -64854,7 +64884,7 @@
         <v>5013</v>
       </c>
     </row>
-    <row r="832" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="832" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A832" s="31" t="s">
         <v>3497</v>
       </c>
@@ -64866,7 +64896,7 @@
         <v>5013</v>
       </c>
     </row>
-    <row r="833" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="833" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A833" s="31" t="s">
         <v>3498</v>
       </c>
@@ -64878,7 +64908,7 @@
         <v>5013</v>
       </c>
     </row>
-    <row r="834" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="834" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A834" s="31" t="s">
         <v>3507</v>
       </c>
@@ -64890,7 +64920,7 @@
         <v>5013</v>
       </c>
     </row>
-    <row r="835" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="835" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A835" s="31" t="s">
         <v>3509</v>
       </c>
@@ -66238,8 +66268,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE9B5EB2-EC05-44CA-88DD-ED44E8058C62}">
   <dimension ref="A1:G1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A471" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A477" sqref="A477"/>
+    <sheetView tabSelected="1" topLeftCell="A754" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A756" sqref="A756"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>